<commit_message>
Correction description Practitioner 41c8475472a0c26358900c151cf838e281be451e
</commit_message>
<xml_diff>
--- a/299-Ajout-de-l'évaluation/ig/StructureDefinition-tddui-practitioner.xlsx
+++ b/299-Ajout-de-l'évaluation/ig/StructureDefinition-tddui-practitioner.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-15T11:45:31+00:00</t>
+    <t>2025-10-15T11:51:21+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,7 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Profil de la ressource FRCorePractitionerProfile permettant de représenter un Profesionnel.</t>
+    <t>Profil de la ressource FRCorePractitionerProfile permettant de représenter un professionnel du médicosocial dans le cadre de TDDUI.</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>